<commit_message>
Added new Action Keyword: clickAlert
</commit_message>
<xml_diff>
--- a/design/ActionKeywords.xlsx
+++ b/design/ActionKeywords.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\81013161\IdeaProjects\bpss-qa-automation\design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\81013567\GitHub\pronghorn\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="81">
   <si>
     <t>Object</t>
   </si>
@@ -122,9 +122,6 @@
     <t>Object:String</t>
   </si>
   <si>
-    <t>Object: String</t>
-  </si>
-  <si>
     <t>Object: String (Absolute File Path)</t>
   </si>
   <si>
@@ -261,6 +258,15 @@
   </si>
   <si>
     <t>select</t>
+  </si>
+  <si>
+    <t>clickAlert</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Alert box actions (yes/no)</t>
   </si>
 </sst>
 </file>
@@ -913,7 +919,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,10 +935,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>1</v>
@@ -957,10 +963,10 @@
         <v>0</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -969,17 +975,17 @@
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -989,7 +995,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
@@ -1003,17 +1009,17 @@
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1025,14 +1031,14 @@
         <v>29</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1044,16 +1050,16 @@
         <v>31</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1062,19 +1068,19 @@
         <v>30</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>30</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1086,10 +1092,10 @@
         <v>0</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>9</v>
@@ -1099,22 +1105,22 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1123,19 +1129,19 @@
         <v>18</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>18</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1144,17 +1150,17 @@
         <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1166,10 +1172,10 @@
         <v>0</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>12</v>
@@ -1178,12 +1184,24 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="6"/>
+      <c r="B14" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
@@ -1205,16 +1223,16 @@
         <v>31</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1226,16 +1244,16 @@
         <v>31</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1244,19 +1262,19 @@
         <v>15</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="E18" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1265,10 +1283,10 @@
         <v>24</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
@@ -1302,19 +1320,19 @@
         <v>16</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1323,19 +1341,19 @@
         <v>17</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1365,7 +1383,7 @@
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3" t="s">
@@ -1380,7 +1398,7 @@
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3" t="s">
@@ -1395,7 +1413,7 @@
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3" t="s">
@@ -1410,7 +1428,7 @@
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3" t="s">
@@ -1424,10 +1442,10 @@
         <v>23</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3" t="s">

</xml_diff>